<commit_message>
new graphs for study design and conflicts of interest
</commit_message>
<xml_diff>
--- a/data/PECO.xlsx
+++ b/data/PECO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PhD\Methods\Citation Anlaysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2286432b\OneDrive - University of Glasgow\R Studio - home folder\Citation network analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_38DD46DEAB8340E946A1EB0A3AD6FDBBC1A607E7" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{151EFEDC-3629-4B1D-A06D-0E8EEDBC317D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7665"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PECO Full" sheetId="3" r:id="rId1"/>
@@ -19,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1100,9 +1095,6 @@
     <t>Nicotine labelling and packaging</t>
   </si>
   <si>
-    <t>Both</t>
-  </si>
-  <si>
     <t xml:space="preserve">No conflicts of interest stated </t>
   </si>
   <si>
@@ -1175,9 +1167,6 @@
     <t xml:space="preserve">systematic review and meta analysis </t>
   </si>
   <si>
-    <t>Monte-Carlo</t>
-  </si>
-  <si>
     <t xml:space="preserve">toxicology </t>
   </si>
   <si>
@@ -1191,12 +1180,18 @@
   </si>
   <si>
     <t>Yan, XS and D'Ruiz, C (2015)</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Both e-cigarrette and pharmaceutical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1567,11 +1562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,22 +1590,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1633,7 +1628,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
@@ -1662,7 +1657,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,10 +1680,10 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1714,7 +1709,7 @@
         <v>160</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1737,10 +1732,10 @@
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1763,10 +1758,10 @@
         <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1789,7 +1784,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>8</v>
@@ -1818,7 +1813,7 @@
         <v>44</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1841,7 +1836,7 @@
         <v>48</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>8</v>
@@ -1867,10 +1862,10 @@
         <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1893,10 +1888,10 @@
         <v>56</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1919,7 +1914,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>8</v>
@@ -1945,7 +1940,7 @@
         <v>64</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>8</v>
@@ -1997,10 +1992,10 @@
         <v>26</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2026,7 +2021,7 @@
         <v>160</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2034,7 +2029,7 @@
         <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>157</v>
@@ -2052,7 +2047,7 @@
         <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2075,7 +2070,7 @@
         <v>81</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>101</v>
@@ -2101,10 +2096,10 @@
         <v>85</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2127,7 +2122,7 @@
         <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>101</v>
@@ -2153,7 +2148,7 @@
         <v>94</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>8</v>
@@ -2208,7 +2203,7 @@
         <v>100</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2260,7 +2255,7 @@
         <v>206</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2283,10 +2278,10 @@
         <v>118</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2312,7 +2307,7 @@
         <v>69</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2320,7 +2315,7 @@
         <v>123</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>11</v>
@@ -2335,7 +2330,7 @@
         <v>61</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>8</v>
@@ -2361,7 +2356,7 @@
         <v>127</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>8</v>
@@ -2387,10 +2382,10 @@
         <v>61</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2416,7 +2411,7 @@
         <v>44</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2439,10 +2434,10 @@
         <v>135</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2465,10 +2460,10 @@
         <v>138</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2491,10 +2486,10 @@
         <v>141</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2528,7 +2523,7 @@
         <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>146</v>
@@ -2546,7 +2541,7 @@
         <v>15</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2569,10 +2564,10 @@
         <v>149</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2595,7 +2590,7 @@
         <v>154</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>101</v>
@@ -2624,7 +2619,7 @@
         <v>160</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2650,7 +2645,7 @@
         <v>100</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2673,10 +2668,10 @@
         <v>166</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2699,10 +2694,10 @@
         <v>170</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2725,7 +2720,7 @@
         <v>173</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>101</v>
@@ -2751,7 +2746,7 @@
         <v>176</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>101</v>
@@ -2777,10 +2772,10 @@
         <v>179</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2803,10 +2798,10 @@
         <v>183</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2829,7 +2824,7 @@
         <v>186</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>101</v>
@@ -2881,10 +2876,10 @@
         <v>193</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2910,7 +2905,7 @@
         <v>69</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2933,10 +2928,10 @@
         <v>202</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2985,10 +2980,10 @@
         <v>209</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3011,7 +3006,7 @@
         <v>213</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>101</v>
@@ -3037,7 +3032,7 @@
         <v>213</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>101</v>
@@ -3063,7 +3058,7 @@
         <v>219</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>101</v>
@@ -3089,7 +3084,7 @@
         <v>222</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>101</v>
@@ -3115,7 +3110,7 @@
         <v>225</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>101</v>
@@ -3170,7 +3165,7 @@
         <v>100</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3196,7 +3191,7 @@
         <v>237</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3222,7 +3217,7 @@
         <v>206</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3245,7 +3240,7 @@
         <v>245</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>8</v>
@@ -3274,7 +3269,7 @@
         <v>69</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3323,10 +3318,10 @@
         <v>254</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3349,10 +3344,10 @@
         <v>257</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3375,10 +3370,10 @@
         <v>260</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3401,7 +3396,7 @@
         <v>263</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>101</v>
@@ -3427,7 +3422,7 @@
         <v>141</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>8</v>
@@ -3479,7 +3474,7 @@
         <v>274</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>101</v>
@@ -3505,10 +3500,10 @@
         <v>277</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3531,10 +3526,10 @@
         <v>281</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3557,7 +3552,7 @@
         <v>285</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>101</v>
@@ -3583,10 +3578,10 @@
         <v>290</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3609,7 +3604,7 @@
         <v>295</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>8</v>
@@ -3635,7 +3630,7 @@
         <v>299</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>101</v>
@@ -3661,10 +3656,10 @@
         <v>303</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3687,10 +3682,10 @@
         <v>193</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3716,7 +3711,7 @@
         <v>100</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3747,7 +3742,7 @@
     </row>
     <row r="84" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>313</v>
@@ -3765,10 +3760,10 @@
         <v>315</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3791,7 +3786,7 @@
         <v>318</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>101</v>
@@ -3820,7 +3815,7 @@
         <v>206</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3843,10 +3838,10 @@
         <v>318</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3869,7 +3864,7 @@
         <v>325</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>101</v>
@@ -3898,7 +3893,7 @@
         <v>160</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3924,7 +3919,7 @@
         <v>332</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3950,7 +3945,7 @@
         <v>69</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3973,10 +3968,10 @@
         <v>338</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3999,7 +3994,7 @@
         <v>213</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>101</v>
@@ -4028,7 +4023,7 @@
         <v>160</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4051,10 +4046,10 @@
         <v>346</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4080,7 +4075,7 @@
         <v>160</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4103,7 +4098,7 @@
         <v>352</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>101</v>
@@ -4129,10 +4124,10 @@
         <v>355</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -4142,6 +4137,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF7793DA0DEC7646B4067AE33236EE6A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a48280fc6c2b4371bf74abb2bee37b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c55d3ce8-937e-4dcf-883e-347e1ce052b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81c33a3acb51a74fa588efcfe98e5c44" ns3:_="">
     <xsd:import namespace="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
@@ -4273,12 +4274,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4289,6 +4284,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8068956F-FE7C-4286-A5F2-2ED11E40F0B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4306,22 +4317,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update of file 13
</commit_message>
<xml_diff>
--- a/data/PECO.xlsx
+++ b/data/PECO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Citation-Network-Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B097B351-8417-45FF-9731-76BC3A5F0504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C068E8E-7BEF-4BD9-B83B-3DEA741830E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,7 +940,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,13 +952,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -976,17 +969,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1013,11 +1001,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1028,19 +1015,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1054,8 +1038,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1370,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2769,25 +2752,25 @@
       <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="10" t="s">
+      <c r="D54" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G54" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="9" t="s">
         <v>80</v>
       </c>
       <c r="I54" s="6"/>
@@ -3988,25 +3971,25 @@
       <c r="A100" s="7">
         <v>99</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" t="s">
         <v>292</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="D100" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E100" s="9" t="s">
+      <c r="D100" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F100" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="G100" s="9" t="s">
+      <c r="G100" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="H100" s="9" t="s">
+      <c r="H100" s="8" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4014,25 +3997,25 @@
       <c r="A101" s="7">
         <v>100</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B101" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D101" s="9" t="s">
+      <c r="D101" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="E101" s="9" t="s">
+      <c r="E101" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F101" s="9" t="s">
+      <c r="F101" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="G101" s="9" t="s">
+      <c r="G101" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="H101" s="9" t="s">
+      <c r="H101" s="8" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4235,18 +4218,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4268,6 +4251,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4281,12 +4272,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated graphs based on 2308 citations
</commit_message>
<xml_diff>
--- a/data/PECO.xlsx
+++ b/data/PECO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marissa\Documents\Citation-Network-Analysis-New\Citation-Network-Analysis-New\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8444D0D-344C-4F71-BBA3-9D15A253E6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12624D7F-84DC-499E-A7DA-CE7B27C30D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="60" windowWidth="9070" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PECO Full" sheetId="3" r:id="rId1"/>
@@ -1371,9 +1371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
+      <selection pane="bottomLeft" activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4131,12 +4131,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF7793DA0DEC7646B4067AE33236EE6A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a48280fc6c2b4371bf74abb2bee37b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c55d3ce8-937e-4dcf-883e-347e1ce052b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81c33a3acb51a74fa588efcfe98e5c44" ns3:_="">
     <xsd:import namespace="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
@@ -4268,16 +4277,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4293,7 +4301,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8068956F-FE7C-4286-A5F2-2ED11E40F0B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4309,12 +4317,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS updates based on new sample
</commit_message>
<xml_diff>
--- a/data/PECO.xlsx
+++ b/data/PECO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marissa\Documents\Citation-Network-Analysis-New\Citation-Network-Analysis-New\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12624D7F-84DC-499E-A7DA-CE7B27C30D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF50190-456F-4A65-93A3-FF8F41CC76A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,9 +405,6 @@
     <t>Literature review</t>
   </si>
   <si>
-    <t>Brown, J et al. (2014c)</t>
-  </si>
-  <si>
     <t xml:space="preserve">England </t>
   </si>
   <si>
@@ -943,6 +940,9 @@
   </si>
   <si>
     <t>e-cigarette use and intiation of other combustible products</t>
+  </si>
+  <si>
+    <t>Brown, J et al. (2014a)</t>
   </si>
 </sst>
 </file>
@@ -1372,8 +1372,8 @@
   <dimension ref="A1:AA102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G102" sqref="G102"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1397,22 +1397,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>8</v>
@@ -1464,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1487,10 +1487,10 @@
         <v>18</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1516,7 +1516,7 @@
         <v>122</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1539,10 +1539,10 @@
         <v>26</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1565,10 +1565,10 @@
         <v>30</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>34</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>8</v>
@@ -1620,7 +1620,7 @@
         <v>37</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1643,7 +1643,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>8</v>
@@ -1669,10 +1669,10 @@
         <v>42</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1695,10 +1695,10 @@
         <v>46</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1721,7 +1721,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>8</v>
@@ -1747,7 +1747,7 @@
         <v>52</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>8</v>
@@ -1799,10 +1799,10 @@
         <v>23</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1828,7 +1828,7 @@
         <v>122</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1836,7 +1836,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>119</v>
@@ -1854,7 +1854,7 @@
         <v>56</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1877,7 +1877,7 @@
         <v>64</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>80</v>
@@ -1903,7 +1903,7 @@
         <v>67</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>80</v>
@@ -1929,7 +1929,7 @@
         <v>70</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>80</v>
@@ -1955,7 +1955,7 @@
         <v>74</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>8</v>
@@ -2010,7 +2010,7 @@
         <v>79</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2033,7 +2033,7 @@
         <v>86</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>80</v>
@@ -2059,10 +2059,10 @@
         <v>88</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2085,10 +2085,10 @@
         <v>93</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2114,7 +2114,7 @@
         <v>56</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2122,7 +2122,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>10</v>
@@ -2137,7 +2137,7 @@
         <v>50</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>8</v>
@@ -2163,7 +2163,7 @@
         <v>99</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>8</v>
@@ -2189,10 +2189,10 @@
         <v>50</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2218,7 +2218,7 @@
         <v>37</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2241,10 +2241,10 @@
         <v>104</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2267,10 +2267,10 @@
         <v>106</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2293,10 +2293,10 @@
         <v>108</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2330,7 +2330,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>111</v>
@@ -2348,7 +2348,7 @@
         <v>14</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2371,10 +2371,10 @@
         <v>113</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2397,7 +2397,7 @@
         <v>117</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>80</v>
@@ -2426,7 +2426,7 @@
         <v>122</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2434,7 +2434,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>123</v>
+        <v>302</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>10</v>
@@ -2443,7 +2443,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>50</v>
@@ -2452,7 +2452,7 @@
         <v>79</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2460,7 +2460,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>25</v>
@@ -2472,13 +2472,13 @@
         <v>17</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -2486,7 +2486,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>119</v>
@@ -2495,16 +2495,16 @@
         <v>5</v>
       </c>
       <c r="E43" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="G43" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2512,7 +2512,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>44</v>
@@ -2524,10 +2524,10 @@
         <v>17</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>80</v>
@@ -2538,7 +2538,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>44</v>
@@ -2550,10 +2550,10 @@
         <v>17</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>80</v>
@@ -2564,7 +2564,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>54</v>
@@ -2576,13 +2576,13 @@
         <v>22</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2590,10 +2590,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>5</v>
@@ -2602,13 +2602,13 @@
         <v>33</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2616,7 +2616,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>119</v>
@@ -2628,10 +2628,10 @@
         <v>60</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>80</v>
@@ -2642,10 +2642,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>11</v>
@@ -2654,7 +2654,7 @@
         <v>33</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>79</v>
@@ -2668,7 +2668,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>4</v>
@@ -2677,16 +2677,16 @@
         <v>5</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="58" x14ac:dyDescent="0.35">
@@ -2694,25 +2694,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>60</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>56</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
@@ -2720,25 +2720,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2746,7 +2746,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>25</v>
@@ -2758,10 +2758,10 @@
         <v>17</v>
       </c>
       <c r="F53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>80</v>
@@ -2772,10 +2772,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>11</v>
@@ -2784,10 +2784,10 @@
         <v>25</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>80</v>
@@ -2821,7 +2821,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>44</v>
@@ -2833,13 +2833,13 @@
         <v>17</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:27" ht="29" x14ac:dyDescent="0.35">
@@ -2847,7 +2847,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>119</v>
@@ -2856,13 +2856,13 @@
         <v>11</v>
       </c>
       <c r="E56" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F56" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="F56" s="7" t="s">
-        <v>160</v>
-      </c>
       <c r="G56" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>80</v>
@@ -2873,7 +2873,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>17</v>
@@ -2885,10 +2885,10 @@
         <v>17</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>80</v>
@@ -2899,10 +2899,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>11</v>
@@ -2911,10 +2911,10 @@
         <v>17</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>80</v>
@@ -2925,7 +2925,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>10</v>
@@ -2937,10 +2937,10 @@
         <v>17</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>80</v>
@@ -2951,7 +2951,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>119</v>
@@ -2963,10 +2963,10 @@
         <v>22</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>80</v>
@@ -2977,7 +2977,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>54</v>
@@ -2989,7 +2989,7 @@
         <v>22</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>56</v>
@@ -3003,10 +3003,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>5</v>
@@ -3015,13 +3015,13 @@
         <v>60</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>79</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="29" x14ac:dyDescent="0.35">
@@ -3029,7 +3029,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>119</v>
@@ -3038,16 +3038,16 @@
         <v>11</v>
       </c>
       <c r="E63" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="G63" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G63" s="7" t="s">
-        <v>177</v>
-      </c>
       <c r="H63" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.35">
@@ -3055,25 +3055,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E64" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="E64" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="F64" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3081,7 +3081,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>90</v>
@@ -3090,13 +3090,13 @@
         <v>11</v>
       </c>
       <c r="E65" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="F65" s="7" t="s">
-        <v>183</v>
-      </c>
       <c r="G65" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>8</v>
@@ -3107,25 +3107,25 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>56</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -3133,13 +3133,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>17</v>
@@ -3148,7 +3148,7 @@
         <v>42</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>80</v>
@@ -3159,7 +3159,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>44</v>
@@ -3171,13 +3171,13 @@
         <v>17</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
@@ -3185,7 +3185,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>44</v>
@@ -3197,13 +3197,13 @@
         <v>17</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3211,7 +3211,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>10</v>
@@ -3223,13 +3223,13 @@
         <v>33</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3237,7 +3237,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>10</v>
@@ -3249,10 +3249,10 @@
         <v>33</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>80</v>
@@ -3263,22 +3263,22 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>108</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>8</v>
@@ -3289,10 +3289,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>11</v>
@@ -3301,10 +3301,10 @@
         <v>17</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>80</v>
@@ -3315,22 +3315,22 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E74" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F74" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="F74" s="7" t="s">
-        <v>203</v>
-      </c>
       <c r="G74" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>80</v>
@@ -3341,7 +3341,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>54</v>
@@ -3353,13 +3353,13 @@
         <v>17</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3367,25 +3367,25 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="D76" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F76" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="G76" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3393,7 +3393,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>54</v>
@@ -3402,13 +3402,13 @@
         <v>66</v>
       </c>
       <c r="E77" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="F77" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="G77" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H77" s="7" t="s">
         <v>80</v>
@@ -3419,25 +3419,25 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="D78" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="7" t="s">
+      <c r="F78" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="F78" s="7" t="s">
-        <v>215</v>
-      </c>
       <c r="G78" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -3445,22 +3445,22 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E79" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="F79" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="G79" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H79" s="7" t="s">
         <v>8</v>
@@ -3471,10 +3471,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C80" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>11</v>
@@ -3483,10 +3483,10 @@
         <v>29</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H80" s="7" t="s">
         <v>80</v>
@@ -3497,25 +3497,25 @@
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -3523,7 +3523,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>4</v>
@@ -3535,13 +3535,13 @@
         <v>29</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3549,25 +3549,25 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C83" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="D83" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>229</v>
       </c>
       <c r="G83" s="7" t="s">
         <v>79</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3575,10 +3575,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C84" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>11</v>
@@ -3587,7 +3587,7 @@
         <v>12</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G84" s="7" t="s">
         <v>79</v>
@@ -3601,7 +3601,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>16</v>
@@ -3610,16 +3610,16 @@
         <v>11</v>
       </c>
       <c r="E85" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="F85" s="7" t="s">
-        <v>234</v>
-      </c>
       <c r="G85" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
@@ -3627,7 +3627,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>44</v>
@@ -3639,10 +3639,10 @@
         <v>39</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>80</v>
@@ -3653,7 +3653,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>44</v>
@@ -3665,13 +3665,13 @@
         <v>17</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -3679,7 +3679,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>44</v>
@@ -3691,13 +3691,13 @@
         <v>17</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3705,7 +3705,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>44</v>
@@ -3717,10 +3717,10 @@
         <v>92</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H89" s="7" t="s">
         <v>80</v>
@@ -3731,25 +3731,25 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>122</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3757,7 +3757,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>17</v>
@@ -3766,16 +3766,16 @@
         <v>11</v>
       </c>
       <c r="E91" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G91" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="F91" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>245</v>
-      </c>
       <c r="H91" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3783,25 +3783,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>60</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>56</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -3809,25 +3809,25 @@
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>44</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
@@ -3835,7 +3835,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>17</v>
@@ -3847,10 +3847,10 @@
         <v>17</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H94" s="7" t="s">
         <v>80</v>
@@ -3861,7 +3861,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>119</v>
@@ -3873,13 +3873,13 @@
         <v>33</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>122</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3887,7 +3887,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>16</v>
@@ -3899,13 +3899,13 @@
         <v>17</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3913,7 +3913,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>119</v>
@@ -3925,13 +3925,13 @@
         <v>33</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>122</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -3939,10 +3939,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>257</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>5</v>
@@ -3951,10 +3951,10 @@
         <v>39</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H98" s="7" t="s">
         <v>80</v>
@@ -3965,7 +3965,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>44</v>
@@ -3977,13 +3977,13 @@
         <v>33</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
@@ -3991,10 +3991,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>11</v>
@@ -4003,10 +4003,10 @@
         <v>33</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H100" s="8" t="s">
         <v>80</v>
@@ -4017,22 +4017,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H101" s="8" t="s">
         <v>80</v>
@@ -4043,22 +4043,22 @@
         <v>101</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>115</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>80</v>
@@ -4140,12 +4140,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF7793DA0DEC7646B4067AE33236EE6A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a48280fc6c2b4371bf74abb2bee37b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c55d3ce8-937e-4dcf-883e-347e1ce052b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81c33a3acb51a74fa588efcfe98e5c44" ns3:_="">
     <xsd:import namespace="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
@@ -4277,6 +4271,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
   <ds:schemaRefs>
@@ -4286,22 +4286,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8068956F-FE7C-4286-A5F2-2ED11E40F0B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4317,4 +4301,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>